<commit_message>
razao e media sem resolver ordenação
</commit_message>
<xml_diff>
--- a/genero/escoma.xlsx
+++ b/genero/escoma.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,19 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Melquias\Desktop\OMT\genero\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7C06ABFD-F626-4FF8-A68B-78667350CAE2}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{8F0BD8CD-1C41-4008-8DA0-A4DFD0AD89A6}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="escoma" sheetId="1" r:id="rId1"/>
+    <sheet name="razão" sheetId="2" r:id="rId2"/>
+    <sheet name="Média" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="14">
   <si>
     <t>Ano</t>
   </si>
@@ -60,12 +62,15 @@
   <si>
     <t>feminino</t>
   </si>
+  <si>
+    <t>Média</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="18" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -196,6 +201,14 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -542,9 +555,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Ênfase1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -601,6 +615,43 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CE2A84FB-808B-4079-8696-D79488C436C1}" name="Tabela1" displayName="Tabela1" ref="A1:J8" totalsRowShown="0">
+  <autoFilter ref="A1:J8" xr:uid="{153EABB8-C11E-4DFE-90A7-5814EC574FC6}"/>
+  <tableColumns count="10">
+    <tableColumn id="1" xr3:uid="{69F9C949-71B3-46C2-8DB2-9F002DB97CD2}" name="Ano"/>
+    <tableColumn id="2" xr3:uid="{9D4C5990-26D5-4071-B2A0-6F303E5347FA}" name="Analfabeto">
+      <calculatedColumnFormula>escoma!B2/escoma!B9</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="3" xr3:uid="{371DECA2-444F-4ED2-B419-E4A2BF24B7FB}" name="Até 5ª Incompleto">
+      <calculatedColumnFormula>escoma!C2/escoma!C9</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" xr3:uid="{ABD06598-5DCE-43D5-A287-185540C2DF08}" name="5ª Completo Fundamental">
+      <calculatedColumnFormula>escoma!D2/escoma!D9</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="5" xr3:uid="{5D63CD27-5FA3-4CBF-B07E-0FD2D71E6AB3}" name="6ª a 9ª Fundamental">
+      <calculatedColumnFormula>escoma!E2/escoma!E9</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" xr3:uid="{BAFC0AE9-ACEB-4B95-BA20-F9391B87D98C}" name="Fundamental Completo">
+      <calculatedColumnFormula>escoma!F2/escoma!F9</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="7" xr3:uid="{0AA33EBE-03F8-4272-8A63-FB58F3CD7FF8}" name="Médio Incompleto">
+      <calculatedColumnFormula>escoma!G2/escoma!G9</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="8" xr3:uid="{8FFC5497-E500-4BFB-9478-B64AA795EBFF}" name="Médio Completo">
+      <calculatedColumnFormula>escoma!H2/escoma!H9</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="9" xr3:uid="{AAAF4046-7082-4BC4-A52A-776763E4FEB6}" name="Superior Incompleto">
+      <calculatedColumnFormula>escoma!I2/escoma!I9</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="10" xr3:uid="{D608FDB8-D255-47C4-99AD-485D05CE8E19}" name="Superior Completo">
+      <calculatedColumnFormula>escoma!J2/escoma!J9</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -899,11 +950,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:N21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N13" sqref="N13"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1434,8 +1485,463 @@
         <v>12</v>
       </c>
     </row>
+    <row r="21" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H21" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6678F60-0C83-40AD-8F2A-4280872D75F1}">
+  <dimension ref="A1:J12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="6.7109375" customWidth="1"/>
+    <col min="2" max="2" width="13" customWidth="1"/>
+    <col min="3" max="3" width="19.140625" customWidth="1"/>
+    <col min="4" max="4" width="26.28515625" customWidth="1"/>
+    <col min="5" max="5" width="20.85546875" customWidth="1"/>
+    <col min="6" max="6" width="24" customWidth="1"/>
+    <col min="7" max="7" width="19.42578125" customWidth="1"/>
+    <col min="8" max="8" width="18" customWidth="1"/>
+    <col min="9" max="9" width="21.28515625" customWidth="1"/>
+    <col min="10" max="10" width="19.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>2018</v>
+      </c>
+      <c r="B2">
+        <f>escoma!B2/escoma!B9</f>
+        <v>8.3209876543209873</v>
+      </c>
+      <c r="C2">
+        <f>escoma!C2/escoma!C9</f>
+        <v>4.9501795332136442</v>
+      </c>
+      <c r="D2">
+        <f>escoma!D2/escoma!D9</f>
+        <v>3.5446540880503146</v>
+      </c>
+      <c r="E2">
+        <f>escoma!E2/escoma!E9</f>
+        <v>4.1319092122830439</v>
+      </c>
+      <c r="F2">
+        <f>escoma!F2/escoma!F9</f>
+        <v>2.3669284770973795</v>
+      </c>
+      <c r="G2">
+        <f>escoma!G2/escoma!G9</f>
+        <v>2.3372154579142403</v>
+      </c>
+      <c r="H2">
+        <f>escoma!H2/escoma!H9</f>
+        <v>1.3164437522381442</v>
+      </c>
+      <c r="I2">
+        <f>escoma!I2/escoma!I9</f>
+        <v>0.76465337697113955</v>
+      </c>
+      <c r="J2">
+        <f>escoma!J2/escoma!J9</f>
+        <v>0.52891328347301481</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2017</v>
+      </c>
+      <c r="B3">
+        <f>escoma!B3/escoma!B10</f>
+        <v>9.5829787234042545</v>
+      </c>
+      <c r="C3">
+        <f>escoma!C3/escoma!C10</f>
+        <v>5.5117845117845121</v>
+      </c>
+      <c r="D3">
+        <f>escoma!D3/escoma!D10</f>
+        <v>3.5973377703826954</v>
+      </c>
+      <c r="E3">
+        <f>escoma!E3/escoma!E10</f>
+        <v>4.024390243902439</v>
+      </c>
+      <c r="F3">
+        <f>escoma!F3/escoma!F10</f>
+        <v>2.3967520554460826</v>
+      </c>
+      <c r="G3">
+        <f>escoma!G3/escoma!G10</f>
+        <v>1.0934289428439636</v>
+      </c>
+      <c r="H3">
+        <f>escoma!H3/escoma!H10</f>
+        <v>1.3079317101144536</v>
+      </c>
+      <c r="I3">
+        <f>escoma!I3/escoma!I10</f>
+        <v>0.84314442413162705</v>
+      </c>
+      <c r="J3">
+        <f>escoma!J3/escoma!J10</f>
+        <v>0.5322109190207881</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2016</v>
+      </c>
+      <c r="B4">
+        <f>escoma!B4/escoma!B11</f>
+        <v>10.917808219178083</v>
+      </c>
+      <c r="C4">
+        <f>escoma!C4/escoma!C11</f>
+        <v>6.7112445414847164</v>
+      </c>
+      <c r="D4">
+        <f>escoma!D4/escoma!D11</f>
+        <v>4.2329916123019569</v>
+      </c>
+      <c r="E4">
+        <f>escoma!E4/escoma!E11</f>
+        <v>3.782209276271566</v>
+      </c>
+      <c r="F4">
+        <f>escoma!F4/escoma!F11</f>
+        <v>2.2765737874097005</v>
+      </c>
+      <c r="G4">
+        <f>escoma!G4/escoma!G11</f>
+        <v>1.0143783583472299</v>
+      </c>
+      <c r="H4">
+        <f>escoma!H4/escoma!H11</f>
+        <v>1.2705186430842654</v>
+      </c>
+      <c r="I4">
+        <f>escoma!I4/escoma!I11</f>
+        <v>0.931091208188631</v>
+      </c>
+      <c r="J4">
+        <f>escoma!J4/escoma!J11</f>
+        <v>0.54930605461731941</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>2015</v>
+      </c>
+      <c r="B5">
+        <f>escoma!B5/escoma!B12</f>
+        <v>9.722419928825623</v>
+      </c>
+      <c r="C5">
+        <f>escoma!C5/escoma!C12</f>
+        <v>5.6738544474393535</v>
+      </c>
+      <c r="D5">
+        <f>escoma!D5/escoma!D12</f>
+        <v>4.3806499813223754</v>
+      </c>
+      <c r="E5">
+        <f>escoma!E5/escoma!E12</f>
+        <v>4.2906183368869932</v>
+      </c>
+      <c r="F5">
+        <f>escoma!F5/escoma!F12</f>
+        <v>2.715059897318882</v>
+      </c>
+      <c r="G5">
+        <f>escoma!G5/escoma!G12</f>
+        <v>1.0602462460268167</v>
+      </c>
+      <c r="H5">
+        <f>escoma!H5/escoma!H12</f>
+        <v>1.2741600187839672</v>
+      </c>
+      <c r="I5">
+        <f>escoma!I5/escoma!I12</f>
+        <v>0.76630193043323547</v>
+      </c>
+      <c r="J5">
+        <f>escoma!J5/escoma!J12</f>
+        <v>0.55510807274039975</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>2014</v>
+      </c>
+      <c r="B6">
+        <f>escoma!B6/escoma!B13</f>
+        <v>33.873684210526314</v>
+      </c>
+      <c r="C6">
+        <f>escoma!C6/escoma!C13</f>
+        <v>7.3360375747224591</v>
+      </c>
+      <c r="D6">
+        <f>escoma!D6/escoma!D13</f>
+        <v>4.7910610465116283</v>
+      </c>
+      <c r="E6">
+        <f>escoma!E6/escoma!E13</f>
+        <v>4.9890159157139653</v>
+      </c>
+      <c r="F6">
+        <f>escoma!F6/escoma!F13</f>
+        <v>1.3905836087063386</v>
+      </c>
+      <c r="G6">
+        <f>escoma!G6/escoma!G13</f>
+        <v>2.7286831175177131</v>
+      </c>
+      <c r="H6">
+        <f>escoma!H6/escoma!H13</f>
+        <v>1.2403650329835747</v>
+      </c>
+      <c r="I6">
+        <f>escoma!I6/escoma!I13</f>
+        <v>0.80277437010474662</v>
+      </c>
+      <c r="J6">
+        <f>escoma!J6/escoma!J13</f>
+        <v>0.5550951304121331</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>2013</v>
+      </c>
+      <c r="B7">
+        <f>escoma!B7/escoma!B14</f>
+        <v>37.673913043478258</v>
+      </c>
+      <c r="C7">
+        <f>escoma!C7/escoma!C14</f>
+        <v>8.3031968031968031</v>
+      </c>
+      <c r="D7">
+        <f>escoma!D7/escoma!D14</f>
+        <v>4.8719193427931291</v>
+      </c>
+      <c r="E7">
+        <f>escoma!E7/escoma!E14</f>
+        <v>5.2157459765115268</v>
+      </c>
+      <c r="F7">
+        <f>escoma!F7/escoma!F14</f>
+        <v>1.3999584889995849</v>
+      </c>
+      <c r="G7">
+        <f>escoma!G7/escoma!G14</f>
+        <v>2.8324879084581811</v>
+      </c>
+      <c r="H7">
+        <f>escoma!H7/escoma!H14</f>
+        <v>1.2392133578034474</v>
+      </c>
+      <c r="I7">
+        <f>escoma!I7/escoma!I14</f>
+        <v>0.7527708437343984</v>
+      </c>
+      <c r="J7">
+        <f>escoma!J7/escoma!J14</f>
+        <v>0.56345376112159606</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>2012</v>
+      </c>
+      <c r="B8">
+        <f>escoma!B8/escoma!B15</f>
+        <v>38.472527472527474</v>
+      </c>
+      <c r="C8">
+        <f>escoma!C8/escoma!C15</f>
+        <v>7.6828212894850711</v>
+      </c>
+      <c r="D8">
+        <f>escoma!D8/escoma!D15</f>
+        <v>4.0141577578734466</v>
+      </c>
+      <c r="E8">
+        <f>escoma!E8/escoma!E15</f>
+        <v>4.7922761849034528</v>
+      </c>
+      <c r="F8">
+        <f>escoma!F8/escoma!F15</f>
+        <v>1.9810169491525425</v>
+      </c>
+      <c r="G8">
+        <f>escoma!G8/escoma!G15</f>
+        <v>2.9102579341495303</v>
+      </c>
+      <c r="H8">
+        <f>escoma!H8/escoma!H15</f>
+        <v>1.1915075883689563</v>
+      </c>
+      <c r="I8">
+        <f>escoma!I8/escoma!I15</f>
+        <v>0.72862603097968215</v>
+      </c>
+      <c r="J8">
+        <f>escoma!J8/escoma!J15</f>
+        <v>0.66450690555198511</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F11" s="2"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H12" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA805D05-CD15-4BD0-A353-66BCB3189895}">
+  <dimension ref="A1:J2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.5703125" customWidth="1"/>
+    <col min="10" max="10" width="18" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2">
+        <f>SUM(razão!B2:B8)/7</f>
+        <v>21.223474178894428</v>
+      </c>
+      <c r="C2">
+        <f>SUM(razão!C2:C8)/7</f>
+        <v>6.5955883859037945</v>
+      </c>
+      <c r="D2">
+        <f>SUM(razão!D2:D8)/7</f>
+        <v>4.2046816570336505</v>
+      </c>
+      <c r="E2">
+        <f>SUM(razão!E2:E8)/7</f>
+        <v>4.4608807352104272</v>
+      </c>
+      <c r="F2">
+        <f>SUM(razão!F2:F8)/7</f>
+        <v>2.0752676091615014</v>
+      </c>
+      <c r="G2">
+        <f>SUM(razão!G2:G8)/7</f>
+        <v>1.9966711378939535</v>
+      </c>
+      <c r="H2">
+        <f>SUM(razão!H2:H8)/7</f>
+        <v>1.2628771576252584</v>
+      </c>
+      <c r="I2">
+        <f>SUM(razão!I2:I8)/7</f>
+        <v>0.79848031207763714</v>
+      </c>
+      <c r="J2">
+        <f>SUM(razão!J2:J8)/7</f>
+        <v>0.56408487527674811</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
 </file>
</xml_diff>